<commit_message>
start course insert into dbf
</commit_message>
<xml_diff>
--- a/ВАКАНСИИ РАЗОСЛАТЬ.xlsx
+++ b/ВАКАНСИИ РАЗОСЛАТЬ.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
   <si>
     <t>Компания</t>
   </si>
@@ -194,6 +194,63 @@
   </si>
   <si>
     <t>ОТКЛОНИЛИ ОТКЛИК</t>
+  </si>
+  <si>
+    <t>ВЫСЛАЛИ ТЕСТОВОЕ, не та пециальность</t>
+  </si>
+  <si>
+    <t>Собеседование прошел</t>
+  </si>
+  <si>
+    <t>мудаки</t>
+  </si>
+  <si>
+    <t>БЭКЭНД-ЭКСПЕРТ</t>
+  </si>
+  <si>
+    <t>VIRON-IT</t>
+  </si>
+  <si>
+    <t>https://jobs.tut.by/vacancy/26812835?query=python%20junior</t>
+  </si>
+  <si>
+    <t>Awem Games</t>
+  </si>
+  <si>
+    <t>https://vk.com/club16451872</t>
+  </si>
+  <si>
+    <t>Хм, им питоха не нужен. Но хз, напиши, чо</t>
+  </si>
+  <si>
+    <t>https://jobs.tut.by/vacancy/26413955?query=Python%20%D1%80%D0%B0%D0%B7%D1%80%D0%B0%D0%B1%D0%BE%D1%82%D1%87%D0%B8%D0%BA</t>
+  </si>
+  <si>
+    <t>*instinctools East Europe labs</t>
+  </si>
+  <si>
+    <t>https://www.instinctools.by/?p=597</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>jobs@instinctools.ru</t>
+  </si>
+  <si>
+    <t>https://jobs.tut.by/vacancy/26885408?query=Python%20%D1%80%D0%B0%D0%B7%D1%80%D0%B0%D0%B1%D0%BE%D1%82%D1%87%D0%B8%D0%BA</t>
+  </si>
+  <si>
+    <t>Gurtam</t>
+  </si>
+  <si>
+    <t>info@gurtam.com</t>
+  </si>
+  <si>
+    <t>собеседование, не прошел</t>
+  </si>
+  <si>
+    <t>собеседование. Не прошел</t>
   </si>
 </sst>
 </file>
@@ -219,12 +276,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -240,12 +315,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -527,15 +607,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -552,24 +632,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -586,7 +672,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -602,8 +688,9 @@
       <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -616,25 +703,31 @@
       <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -647,8 +740,9 @@
       <c r="E7" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -661,8 +755,9 @@
       <c r="G8" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -675,22 +770,28 @@
       <c r="E9" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="D10" s="3"/>
+      <c r="E10" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -710,7 +811,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -720,8 +821,9 @@
       <c r="E12" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -731,6 +833,67 @@
       <c r="E13" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -758,8 +921,15 @@
     <hyperlink ref="E12" r:id="rId22"/>
     <hyperlink ref="E13" r:id="rId23"/>
     <hyperlink ref="C13" r:id="rId24"/>
+    <hyperlink ref="C16" r:id="rId25"/>
+    <hyperlink ref="E16" r:id="rId26"/>
+    <hyperlink ref="C17" r:id="rId27"/>
+    <hyperlink ref="D17" r:id="rId28"/>
+    <hyperlink ref="E17" r:id="rId29"/>
+    <hyperlink ref="C18" r:id="rId30"/>
+    <hyperlink ref="E18" r:id="rId31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId25"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>